<commit_message>
Objedinjen tekst sa novom 1.0.9.9.9.9 zakrpom
</commit_message>
<xml_diff>
--- a/Lista zaduženja_StalkerSoup.xlsx
+++ b/Lista zaduženja_StalkerSoup.xlsx
@@ -764,13 +764,13 @@
     <t>string_table_text_after_1100</t>
   </si>
   <si>
-    <t>150 - komada</t>
-  </si>
-  <si>
     <t>stable_dialogs_tb3d_2</t>
   </si>
   <si>
-    <t>11 - komada</t>
+    <t>9- komada</t>
+  </si>
+  <si>
+    <t>152 - komada</t>
   </si>
 </sst>
 </file>
@@ -1536,7 +1536,7 @@
     <xf numFmtId="49" fontId="20" fillId="8" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1689,7 +1689,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2036,8 +2036,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S197"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H130" sqref="H130:K130"/>
+    <sheetView tabSelected="1" topLeftCell="A86" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C121" sqref="C121:F122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2360,13 +2360,13 @@
         <v>7</v>
       </c>
       <c r="M14" s="79" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="N14" s="80"/>
       <c r="O14" s="80"/>
       <c r="P14" s="80"/>
       <c r="Q14" s="23">
-        <v>175</v>
+        <v>98</v>
       </c>
       <c r="R14" s="1"/>
     </row>
@@ -2967,11 +2967,15 @@
       <c r="L32" s="22">
         <v>5</v>
       </c>
-      <c r="M32" s="81"/>
+      <c r="M32" s="81" t="s">
+        <v>173</v>
+      </c>
       <c r="N32" s="82"/>
       <c r="O32" s="82"/>
       <c r="P32" s="83"/>
-      <c r="Q32" s="27"/>
+      <c r="Q32" s="27">
+        <v>175</v>
+      </c>
       <c r="R32" s="1"/>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.25">
@@ -3383,13 +3387,13 @@
         <v>1</v>
       </c>
       <c r="M46" s="79" t="s">
-        <v>86</v>
+        <v>170</v>
       </c>
       <c r="N46" s="80"/>
       <c r="O46" s="80"/>
       <c r="P46" s="80"/>
       <c r="Q46" s="23">
-        <v>148</v>
+        <v>80</v>
       </c>
       <c r="R46" s="1"/>
     </row>
@@ -4183,11 +4187,15 @@
       <c r="G72" s="21">
         <v>7</v>
       </c>
-      <c r="H72" s="29"/>
+      <c r="H72" s="29" t="s">
+        <v>86</v>
+      </c>
       <c r="I72" s="29"/>
       <c r="J72" s="29"/>
       <c r="K72" s="29"/>
-      <c r="L72" s="22"/>
+      <c r="L72" s="22">
+        <v>148</v>
+      </c>
       <c r="M72" s="30"/>
       <c r="N72" s="31"/>
       <c r="O72" s="31"/>
@@ -5117,15 +5125,11 @@
       <c r="G107" s="21">
         <v>42</v>
       </c>
-      <c r="H107" s="29" t="s">
-        <v>189</v>
-      </c>
+      <c r="H107" s="29"/>
       <c r="I107" s="29"/>
       <c r="J107" s="29"/>
       <c r="K107" s="29"/>
-      <c r="L107" s="22">
-        <v>18</v>
-      </c>
+      <c r="L107" s="22"/>
       <c r="M107" s="30"/>
       <c r="N107" s="31"/>
       <c r="O107" s="31"/>
@@ -5193,14 +5197,14 @@
         <f t="shared" si="3"/>
         <v>4</v>
       </c>
-      <c r="C110" s="28" t="s">
-        <v>170</v>
+      <c r="C110" s="43" t="s">
+        <v>171</v>
       </c>
       <c r="D110" s="28"/>
       <c r="E110" s="28"/>
       <c r="F110" s="28"/>
       <c r="G110" s="21">
-        <v>80</v>
+        <v>63</v>
       </c>
       <c r="H110" s="29"/>
       <c r="I110" s="29"/>
@@ -5220,14 +5224,14 @@
         <f t="shared" si="3"/>
         <v>5</v>
       </c>
-      <c r="C111" s="28" t="s">
-        <v>171</v>
+      <c r="C111" s="43" t="s">
+        <v>188</v>
       </c>
       <c r="D111" s="28"/>
       <c r="E111" s="28"/>
       <c r="F111" s="28"/>
       <c r="G111" s="21">
-        <v>63</v>
+        <v>18</v>
       </c>
       <c r="H111" s="29"/>
       <c r="I111" s="29"/>
@@ -5302,13 +5306,13 @@
         <v>8</v>
       </c>
       <c r="C114" s="43" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="D114" s="28"/>
       <c r="E114" s="28"/>
       <c r="F114" s="28"/>
       <c r="G114" s="21">
-        <v>98</v>
+        <v>77</v>
       </c>
       <c r="H114" s="29"/>
       <c r="I114" s="29"/>
@@ -5355,15 +5359,11 @@
         <f t="shared" si="3"/>
         <v>10</v>
       </c>
-      <c r="C116" s="28" t="s">
-        <v>176</v>
-      </c>
+      <c r="C116" s="28"/>
       <c r="D116" s="28"/>
       <c r="E116" s="28"/>
       <c r="F116" s="28"/>
-      <c r="G116" s="21">
-        <v>77</v>
-      </c>
+      <c r="G116" s="21"/>
       <c r="H116" s="29"/>
       <c r="I116" s="29"/>
       <c r="J116" s="29"/>
@@ -5390,7 +5390,7 @@
       <c r="I117" s="86"/>
       <c r="J117" s="88">
         <f ca="1" xml:space="preserve"> TODAY()</f>
-        <v>42304</v>
+        <v>42363</v>
       </c>
       <c r="K117" s="88"/>
       <c r="L117" s="88"/>
@@ -5471,7 +5471,7 @@
       <c r="A121" s="1"/>
       <c r="B121" s="12"/>
       <c r="C121" s="44" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="D121" s="45"/>
       <c r="E121" s="45"/>
@@ -5485,7 +5485,7 @@
       <c r="K121" s="46"/>
       <c r="L121" s="50"/>
       <c r="M121" s="44" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="N121" s="45"/>
       <c r="O121" s="45"/>
@@ -5560,7 +5560,7 @@
       <c r="B125" s="12"/>
       <c r="C125" s="35">
         <f>SUM(G14:G43,L14:L43,Q21:Q43,G46:G75,L46:L75,Q53:Q75,G78:G87,L78:L87,Q85:Q87,G90:G104,L90:L104,Q97:Q104)</f>
-        <v>3272</v>
+        <v>3595</v>
       </c>
       <c r="D125" s="36"/>
       <c r="E125" s="39" t="s">
@@ -5570,7 +5570,7 @@
       <c r="G125" s="50"/>
       <c r="H125" s="35">
         <f>SUM(Q14:Q15,Q18:Q20,Q46:Q47,Q50:Q52,Q78:Q79,Q82:Q84,Q90:Q91,Q94:Q96)</f>
-        <v>353</v>
+        <v>208</v>
       </c>
       <c r="I125" s="36"/>
       <c r="J125" s="39" t="s">
@@ -5580,7 +5580,7 @@
       <c r="L125" s="50"/>
       <c r="M125" s="35">
         <f>SUM(G107:G116,L107:L116)</f>
-        <v>1137</v>
+        <v>959</v>
       </c>
       <c r="N125" s="36"/>
       <c r="O125" s="39" t="s">

</xml_diff>